<commit_message>
add publication costs 2022, set background color of charts
</commit_message>
<xml_diff>
--- a/raw_data/oa_costs.xlsx
+++ b/raw_data/oa_costs.xlsx
@@ -61,9 +61,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,9 +90,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -377,11 +373,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -390,7 +384,7 @@
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -406,11 +400,14 @@
       <c r="E1">
         <v>2021</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1">
+        <v>2022</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -427,10 +424,13 @@
         <v>726339.07</v>
       </c>
       <c r="F2" s="1">
-        <v>1629587.71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>891555.52</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2521143.23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -447,10 +447,13 @@
         <v>498362.36</v>
       </c>
       <c r="F3" s="1">
-        <v>1211074.28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>484439.77</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1695514.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -467,10 +470,13 @@
         <v>357886.69</v>
       </c>
       <c r="F4" s="1">
-        <v>896992.38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>96717.22</v>
+      </c>
+      <c r="G4" s="1">
+        <v>993709.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -487,10 +493,13 @@
         <v>245278.91</v>
       </c>
       <c r="F5" s="1">
-        <v>540145.77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>251230.77</v>
+      </c>
+      <c r="G5" s="1">
+        <v>791376.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -507,10 +516,13 @@
         <v>16858.55</v>
       </c>
       <c r="F6" s="1">
-        <v>184827.17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26631.98</v>
+      </c>
+      <c r="G6" s="1">
+        <v>211459.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -527,10 +539,13 @@
         <v>16001.15</v>
       </c>
       <c r="F7" s="1">
-        <v>73762.070000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9695.11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>83457.179999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -547,10 +562,13 @@
         <v>25524.29</v>
       </c>
       <c r="F8" s="1">
-        <v>63494.82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23695.11</v>
+      </c>
+      <c r="G8" s="1">
+        <v>87189.93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -567,10 +585,13 @@
         <v>20928.28</v>
       </c>
       <c r="F9" s="1">
-        <v>57178.559999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9093.98</v>
+      </c>
+      <c r="G9" s="1">
+        <v>66272.539999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -587,10 +608,13 @@
         <v>21916.48</v>
       </c>
       <c r="F10" s="1">
-        <v>47688.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5218.1499999999996</v>
+      </c>
+      <c r="G10" s="1">
+        <v>52907.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -607,78 +631,147 @@
         <v>12776.48</v>
       </c>
       <c r="F11" s="1">
-        <v>33626.269999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+        <v>12486.67</v>
+      </c>
+      <c r="G11" s="1">
+        <v>46112.94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>